<commit_message>
Update NIIT-CISCU-US - 25MMS2903-Attendance Roster_Splunk Basics_03-05 September.xlsx
</commit_message>
<xml_diff>
--- a/NIIT-CISCU-US - 25MMS2903-Attendance Roster_Splunk Basics_03-05 September.xlsx
+++ b/NIIT-CISCU-US - 25MMS2903-Attendance Roster_Splunk Basics_03-05 September.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivek\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VK_GIT\SPLK_CISCO_03_09_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E35EE94-4613-46ED-BFED-78A8E94F4875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8333691-2734-46C2-A91F-D3E3FF29F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>Start Date</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Cloud Lab URL as follows : https://cloud.cdp.rpsconsulting.in/console/#/</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -646,22 +649,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -946,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,10 +962,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,7 +1052,9 @@
       <c r="B12" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" s="17"/>
       <c r="E12" s="11"/>
     </row>
@@ -1060,7 +1065,9 @@
       <c r="B13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D13" s="18"/>
       <c r="E13" s="12"/>
     </row>
@@ -1071,7 +1078,9 @@
       <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D14" s="18"/>
       <c r="E14" s="12"/>
     </row>
@@ -1082,7 +1091,9 @@
       <c r="B15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="18"/>
       <c r="E15" s="12"/>
     </row>
@@ -1093,7 +1104,9 @@
       <c r="B16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D16" s="18"/>
       <c r="E16" s="12"/>
     </row>
@@ -1104,7 +1117,9 @@
       <c r="B17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D17" s="18"/>
       <c r="E17" s="12"/>
     </row>
@@ -1115,7 +1130,9 @@
       <c r="B18" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12"/>
     </row>
@@ -1126,7 +1143,9 @@
       <c r="B19" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="23"/>
+      <c r="C19" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D19" s="18"/>
       <c r="E19" s="12"/>
     </row>
@@ -1137,7 +1156,9 @@
       <c r="B20" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="23"/>
+      <c r="C20" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D20" s="18"/>
       <c r="E20" s="12"/>
     </row>
@@ -1148,7 +1169,9 @@
       <c r="B21" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="23"/>
+      <c r="C21" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D21" s="18"/>
       <c r="E21" s="12"/>
     </row>
@@ -1159,7 +1182,9 @@
       <c r="B22" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="24"/>
+      <c r="C22" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="D22" s="19"/>
       <c r="E22" s="13"/>
     </row>
@@ -1170,7 +1195,9 @@
       <c r="B23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="25"/>
+      <c r="C23" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="D23" s="20"/>
       <c r="E23" s="14"/>
     </row>
@@ -1203,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF14E1E-7210-40A5-9668-610A3ED4D61E}">
   <dimension ref="A3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -1215,206 +1242,206 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="36" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39" t="s">
+      <c r="C11" s="35"/>
+      <c r="D11" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="36" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="39" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="36"/>
+      <c r="F17" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>